<commit_message>
1. Update Helper :    - Helper_API.php 2. Update API Document    - API-List.xlsx    - [ TEMPLATE - transaction.delete.... ].docx    - transaction.delete.master.setBloodAglutinogenType (v.1-r.0).docx    - transaction.initialize.master.setBusinessDocumentType (v.1-r.0).docx    - transaction.initialize.master.setCitizenIdentity (v.1-r.0).docx    - transaction.initialize.master.setCountry (v.1-r.0).docx    - transaction.initialize.master.setCountryAdministrativeAreaLevel1 (v.1-r.0).docx    - transaction.initialize.master.setCountryAdministrativeAreaLevel2 (v.1-r.0).docx    - transaction.initialize.master.setCountryAdministrativeAreaLevel3 (v.1-r.0).docx    - transaction.initialize.master.setCountryAdministrativeAreaLevel4 (v.1-r.0).docx    - [ TEMPLATE - transaction.undelete.... ].docx    - transaction.undelete.master.setBloodAglutinogenType (v.1-r.0).docx 3. Update JSON Request Schema 4. Update API Engine
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -173,6 +173,102 @@
   </si>
   <si>
     <t>Mendapatkan Daftar Merk Dagang dari Data Master</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setBloodAglutinogenType</t>
+  </si>
+  <si>
+    <t>Menghapus data jenis golongan darah</t>
+  </si>
+  <si>
+    <t>transaction.undelete.master.setBloodAglutinogenType</t>
+  </si>
+  <si>
+    <t>Membatalkan penghapusan data jenis golongan darah</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setBloodAglutinogenType</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Jenis Golongan Darah</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setBusinessDocumentType</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Jenis Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Identitas Penduduk</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setCitizenIdentity</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setCountry</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Negara</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setCountryAdministrativeAreaLevel1</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setCountryAdministrativeAreaLevel2</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setCountryAdministrativeAreaLevel3</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setCountryAdministrativeAreaLevel4</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Kabupaten / Kota (Daerah Tingkat 2)</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Propinsi (Daerah Tingkat 1)</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Kelurahan / Desa (Daerah Tingkat 4)</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Kecamatan (Daerah Tingkat 3)</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setCurrency</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setDayOffNational</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setDayOffGovernmentPolicy</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setGoodsModel</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setGoodsType</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setPeriod</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setPerson</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setPersonAccountEMail</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setPersonGender</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setProductType</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setReligion</t>
+  </si>
+  <si>
+    <t>transaction.initialize.master.setTradeMark</t>
   </si>
 </sst>
 </file>
@@ -208,7 +304,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +323,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="3"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="3" tint="0.80001220740379042"/>
+        </stop>
+        <stop position="1">
+          <color theme="3"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -318,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -352,6 +461,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -657,13 +772,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C34"/>
+  <dimension ref="B1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -707,9 +822,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="4"/>
+    <row r="6" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -719,9 +834,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="4"/>
+    <row r="8" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
@@ -731,9 +846,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="4"/>
+    <row r="10" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
@@ -743,177 +858,341 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="4"/>
+    <row r="12" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>82</v>
+      </c>
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="12"/>
+      <c r="C55" s="13"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="12"/>
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C58" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="8"/>
-      <c r="C34" s="6"/>
+    <row r="59" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="8"/>
+      <c r="C59" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Pertanggal 12 November 2020
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -178,15 +178,9 @@
     <t>transaction.delete.master.setBloodAglutinogenType</t>
   </si>
   <si>
-    <t>Menghapus data jenis golongan darah</t>
-  </si>
-  <si>
     <t>transaction.undelete.master.setBloodAglutinogenType</t>
   </si>
   <si>
-    <t>Membatalkan penghapusan data jenis golongan darah</t>
-  </si>
-  <si>
     <t>transaction.initialize.master.setBloodAglutinogenType</t>
   </si>
   <si>
@@ -272,6 +266,48 @@
   </si>
   <si>
     <t>Menginisialisasi Data Mata Uang</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Hari Libur Kebijakan Pemerintah</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Hari Libur Nasional</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Model Barang</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Jenis Barang</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Periode dari Data Master</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Periode</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Orang</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Akun EMail Orang</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Jenis Kelamin Orang</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Jenis Produk</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Agama</t>
+  </si>
+  <si>
+    <t>Menginisialisasi Data Merk Dagang</t>
+  </si>
+  <si>
+    <t>Menghapus Data Jenis Golongan Darah</t>
+  </si>
+  <si>
+    <t>Membatalkan Penghapusan Data Jenis Golongan Darah</t>
   </si>
 </sst>
 </file>
@@ -778,10 +814,10 @@
   <dimension ref="B1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -870,7 +906,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -879,141 +915,163 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="4"/>
+        <v>75</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="4"/>
+        <v>79</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="35" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="12"/>
@@ -1112,7 +1170,7 @@
         <v>38</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
@@ -1177,10 +1235,10 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update API Engine and Documentation
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>Membatalkan Penghapusan Data Jenis Golongan Darah</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setBusinessDocument</t>
+  </si>
+  <si>
+    <t>Menghapus Data Dokumen Bisnis</t>
   </si>
 </sst>
 </file>
@@ -811,13 +817,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C59"/>
+  <dimension ref="B1:C82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -909,353 +915,449 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>89</v>
-      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>47</v>
+        <v>76</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="12"/>
-      <c r="C55" s="13"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="12"/>
+      <c r="C58" s="13"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="12"/>
+      <c r="C78" s="13"/>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C79" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="12"/>
-      <c r="C57" s="13"/>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
+    <row r="80" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="12"/>
+      <c r="C80" s="13"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C81" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="8"/>
-      <c r="C59" s="6"/>
+    <row r="82" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="8"/>
+      <c r="C82" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Pertanggal 13 November 2020
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -314,6 +314,24 @@
   </si>
   <si>
     <t>Menghapus Data Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setBusinessDocumentType</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setCountry</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setCitizenIdentity</t>
+  </si>
+  <si>
+    <t>Menghapus Data Jenis Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>Menghapus Data Identitas Penduduk</t>
+  </si>
+  <si>
+    <t>Menghapus Data Negara</t>
   </si>
 </sst>
 </file>
@@ -820,10 +838,10 @@
   <dimension ref="B1:C82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -924,16 +942,28 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>

</xml_diff>

<commit_message>
Penambahan API Engine dan Update Keterangan pada API Engine
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>Menghapus Data Negara</t>
+  </si>
+  <si>
+    <t>transaction.synchronize.project.setProject</t>
   </si>
 </sst>
 </file>
@@ -835,13 +838,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C82"/>
+  <dimension ref="B1:C84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1367,10 +1370,10 @@
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1379,15 +1382,27 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="12"/>
+      <c r="C82" s="13"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="8"/>
-      <c r="C82" s="6"/>
+    <row r="84" spans="2:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="8"/>
+      <c r="C84" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Penambahan API Engine dan Dokumentasi
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
+++ b/Documentation/Documents/Blue Print/API Documents/API-List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -338,6 +338,30 @@
   </si>
   <si>
     <t>Memutakhirkan Data Jenis Golongan Darah</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setCountryAdministrativeAreaLevel1</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setCountryAdministrativeAreaLevel2</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setCountryAdministrativeAreaLevel3</t>
+  </si>
+  <si>
+    <t>transaction.delete.master.setCountryAdministrativeAreaLevel4</t>
+  </si>
+  <si>
+    <t>Menghapusi Data Propinsi (Daerah Tingkat 1)</t>
+  </si>
+  <si>
+    <t>Menghapusi Data Kabupaten / Kota (Daerah Tingkat 2)</t>
+  </si>
+  <si>
+    <t>Menghapusi Data Kecamatan (Daerah Tingkat 3)</t>
+  </si>
+  <si>
+    <t>Menghapusi Data Kelurahan / Desa (Daerah Tingkat 4)</t>
   </si>
 </sst>
 </file>
@@ -844,10 +868,10 @@
   <dimension ref="B1:C84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C72" sqref="C72"/>
+      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -972,20 +996,36 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>

</xml_diff>